<commit_message>
Added 1 row to xls file
</commit_message>
<xml_diff>
--- a/config/CHC_Data_Design_Template.xlsx
+++ b/config/CHC_Data_Design_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakshibangre\Documents\CICD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitarora6\Desktop\Projects\1. Clients\9. Sanofi\CICD\Demo_Project\snowflake_demo\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DAC60F-77A5-43D1-A004-115D61FAB206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1481F902-2946-47D7-AC85-15795BAF0CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="747" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="747" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="95" r:id="rId1"/>
@@ -35,7 +35,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">STAGE!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9006" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9012" uniqueCount="1135">
   <si>
     <t>Overview</t>
   </si>
@@ -4146,12 +4145,18 @@
   <si>
     <t>DROP</t>
   </si>
+  <si>
+    <t>TEST_ID</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38">
+  <fonts count="39">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4406,6 +4411,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -4673,7 +4685,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4972,13 +4984,31 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -5031,6 +5061,412 @@
     <cellStyle name="Normal 3" xfId="46" xr:uid="{D95D2927-27F6-44B4-BFEA-7178A3871294}"/>
   </cellStyles>
   <dxfs count="182">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5461,34 +5897,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5926,104 +6334,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -6455,104 +6765,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -7034,104 +7246,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -8062,90 +8176,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF6600"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -8476,87 +8506,87 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:AH16" totalsRowShown="0" headerRowDxfId="161" dataDxfId="159" headerRowBorderDxfId="160" tableBorderDxfId="158" totalsRowBorderDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:AH16" totalsRowShown="0" headerRowDxfId="173" dataDxfId="171" headerRowBorderDxfId="172" tableBorderDxfId="170" totalsRowBorderDxfId="169">
   <tableColumns count="34">
-    <tableColumn id="20" xr3:uid="{75E059F1-4F3B-4AB7-88F1-A2FF0C4D1ABD}" name="FEED_TYPE" dataDxfId="156"/>
-    <tableColumn id="17" xr3:uid="{87C56FC3-0BA8-47FE-8190-5265289A5345}" name="FEED_ID" dataDxfId="155"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SOURCE_FEED_NAME" dataDxfId="154"/>
-    <tableColumn id="37" xr3:uid="{F45A13EE-DD2E-4CBB-9E7B-99C852321A1C}" name="TARGET_FEED_NAME" dataDxfId="153">
+    <tableColumn id="20" xr3:uid="{75E059F1-4F3B-4AB7-88F1-A2FF0C4D1ABD}" name="FEED_TYPE" dataDxfId="168"/>
+    <tableColumn id="17" xr3:uid="{87C56FC3-0BA8-47FE-8190-5265289A5345}" name="FEED_ID" dataDxfId="167"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SOURCE_FEED_NAME" dataDxfId="166"/>
+    <tableColumn id="37" xr3:uid="{F45A13EE-DD2E-4CBB-9E7B-99C852321A1C}" name="TARGET_FEED_NAME" dataDxfId="165">
       <calculatedColumnFormula>"T_"&amp;Table1[[#This Row],[SOURCE_FEED_NAME]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{9F482604-2D4F-4C66-A9F1-F70B0426BCB7}" name="DESCRIPTION" dataDxfId="152"/>
-    <tableColumn id="25" xr3:uid="{790E50EE-2B1F-4610-AD3A-3F7E17BAC034}" name="FEED_PROCESSING_GROUP" dataDxfId="151"/>
-    <tableColumn id="27" xr3:uid="{AB2808F9-F13B-E247-8A3C-F8F8D940435F}" name="FEED_PROCESSING_ORDER" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PRIORITY" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{F54228EE-54DF-40B8-93C1-65F010B60F3E}" name="CADENCE" dataDxfId="148"/>
-    <tableColumn id="9" xr3:uid="{A03A9999-94EA-43FF-8BB8-C8D1934B865E}" name="INITIAL_LOAD_REQUIRED" dataDxfId="147"/>
-    <tableColumn id="21" xr3:uid="{97133C34-3B58-4627-9669-FEE1B4BD36BE}" name="INITIAL_LOAD_DATA_SCOPE" dataDxfId="146"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="LOAD_TYPE" dataDxfId="145"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="INCREMENTAL_FEED_CRITERIA" dataDxfId="144"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="PERISCOPE_LOAD_TYPE" dataDxfId="143"/>
-    <tableColumn id="44" xr3:uid="{EADB6304-1ED1-4552-B5B7-273FDFCD40EC}" name="FEED_LOAD_LOGIC" dataDxfId="142"/>
-    <tableColumn id="22" xr3:uid="{F2E9683E-F1B4-AD41-B4E0-6F1B8FFA7554}" name="ALLOW_MICROBATCH_LOAD" dataDxfId="141"/>
-    <tableColumn id="31" xr3:uid="{F6FB8BC7-A22B-0842-9803-54AFF355D2FE}" name="MICROBATCH_LOAD_LOGIC" dataDxfId="140"/>
-    <tableColumn id="40" xr3:uid="{F47F2EBC-41FF-FA42-890C-9EE4B78A4EF5}" name="MICROBATCH_FAILRE_PROCESSING_MODE" dataDxfId="139"/>
-    <tableColumn id="39" xr3:uid="{FB5D3B31-8DED-47D9-80DF-2DA522326201}" name="SCD_KEY_1" dataDxfId="138"/>
-    <tableColumn id="42" xr3:uid="{C3D25612-8C8C-4687-AD5C-5B5D1D255217}" name="SCD_KEY_2" dataDxfId="137"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="FILE_NAME_FORMAT_TXT" dataDxfId="136">
+    <tableColumn id="23" xr3:uid="{9F482604-2D4F-4C66-A9F1-F70B0426BCB7}" name="DESCRIPTION" dataDxfId="164"/>
+    <tableColumn id="25" xr3:uid="{790E50EE-2B1F-4610-AD3A-3F7E17BAC034}" name="FEED_PROCESSING_GROUP" dataDxfId="163"/>
+    <tableColumn id="27" xr3:uid="{AB2808F9-F13B-E247-8A3C-F8F8D940435F}" name="FEED_PROCESSING_ORDER" dataDxfId="162"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="PRIORITY" dataDxfId="161"/>
+    <tableColumn id="5" xr3:uid="{F54228EE-54DF-40B8-93C1-65F010B60F3E}" name="CADENCE" dataDxfId="160"/>
+    <tableColumn id="9" xr3:uid="{A03A9999-94EA-43FF-8BB8-C8D1934B865E}" name="INITIAL_LOAD_REQUIRED" dataDxfId="159"/>
+    <tableColumn id="21" xr3:uid="{97133C34-3B58-4627-9669-FEE1B4BD36BE}" name="INITIAL_LOAD_DATA_SCOPE" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="LOAD_TYPE" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="INCREMENTAL_FEED_CRITERIA" dataDxfId="156"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="PERISCOPE_LOAD_TYPE" dataDxfId="155"/>
+    <tableColumn id="44" xr3:uid="{EADB6304-1ED1-4552-B5B7-273FDFCD40EC}" name="FEED_LOAD_LOGIC" dataDxfId="154"/>
+    <tableColumn id="22" xr3:uid="{F2E9683E-F1B4-AD41-B4E0-6F1B8FFA7554}" name="ALLOW_MICROBATCH_LOAD" dataDxfId="153"/>
+    <tableColumn id="31" xr3:uid="{F6FB8BC7-A22B-0842-9803-54AFF355D2FE}" name="MICROBATCH_LOAD_LOGIC" dataDxfId="152"/>
+    <tableColumn id="40" xr3:uid="{F47F2EBC-41FF-FA42-890C-9EE4B78A4EF5}" name="MICROBATCH_FAILRE_PROCESSING_MODE" dataDxfId="151"/>
+    <tableColumn id="39" xr3:uid="{FB5D3B31-8DED-47D9-80DF-2DA522326201}" name="SCD_KEY_1" dataDxfId="150"/>
+    <tableColumn id="42" xr3:uid="{C3D25612-8C8C-4687-AD5C-5B5D1D255217}" name="SCD_KEY_2" dataDxfId="149"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="FILE_NAME_FORMAT_TXT" dataDxfId="148">
       <calculatedColumnFormula>""&amp;Table1[[#This Row],[SOURCE_FEED_NAME]]&amp;"_YYYYMMDDHHMI.csv"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="FILE_NAME_FORMAT" dataDxfId="135">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="FILE_NAME_FORMAT" dataDxfId="147">
       <calculatedColumnFormula>"US_ALL_HYG_"&amp;Table1[[#This Row],[SOURCE_FEED_NAME]]&amp;"_YYYYMMDDHHMI.csv"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{6E63611C-E693-7143-AE39-8A1336E7A00C}" name="CHUNK_MASK" dataDxfId="134"/>
-    <tableColumn id="33" xr3:uid="{874AC529-F9AD-C743-B62D-54B0350B6CAC}" name="FILE_HEADER_ROW" dataDxfId="133"/>
-    <tableColumn id="12" xr3:uid="{F6BADD41-99BB-4946-B23C-0CCA2D35C051}" name="FILE_COLUMN_DELIMITER" dataDxfId="132"/>
-    <tableColumn id="29" xr3:uid="{2AE6156D-9FCD-014B-99CB-B0C58A59B41C}" name="FIELDS_ENCLOSED" dataDxfId="131"/>
-    <tableColumn id="34" xr3:uid="{CDCABEF9-BAF0-C043-AACE-67A1206A915D}" name="ESCAPE_CHARACTER" dataDxfId="130"/>
-    <tableColumn id="28" xr3:uid="{B74F90B2-DAF7-B94F-8284-1EEA400EF1FB}" name="DATE_FORMAT" dataDxfId="129"/>
-    <tableColumn id="35" xr3:uid="{03B4F8A1-AD12-8341-A343-173B2E180299}" name="DATETIME_FORMAT" dataDxfId="128"/>
-    <tableColumn id="36" xr3:uid="{DABEE994-4152-4DD6-ABEC-EB95AD8FE941}" name="FEED_RELEVANCE" dataDxfId="127"/>
-    <tableColumn id="38" xr3:uid="{78F40883-259F-1949-8F96-1FAFC8B1302C}" name="ENCRYPTED" dataDxfId="126"/>
-    <tableColumn id="26" xr3:uid="{420FC220-FD78-47EB-971E-A87F3D459433}" name="ESTIMATED_VOLUME_IN_GB" dataDxfId="125"/>
-    <tableColumn id="1" xr3:uid="{9F60E835-17EA-402E-BE58-F664166419BB}" name="PROMO" dataDxfId="124"/>
-    <tableColumn id="24" xr3:uid="{05342558-0B99-49EA-816A-D0DF857E4361}" name="PRICE" dataDxfId="123"/>
+    <tableColumn id="32" xr3:uid="{6E63611C-E693-7143-AE39-8A1336E7A00C}" name="CHUNK_MASK" dataDxfId="146"/>
+    <tableColumn id="33" xr3:uid="{874AC529-F9AD-C743-B62D-54B0350B6CAC}" name="FILE_HEADER_ROW" dataDxfId="145"/>
+    <tableColumn id="12" xr3:uid="{F6BADD41-99BB-4946-B23C-0CCA2D35C051}" name="FILE_COLUMN_DELIMITER" dataDxfId="144"/>
+    <tableColumn id="29" xr3:uid="{2AE6156D-9FCD-014B-99CB-B0C58A59B41C}" name="FIELDS_ENCLOSED" dataDxfId="143"/>
+    <tableColumn id="34" xr3:uid="{CDCABEF9-BAF0-C043-AACE-67A1206A915D}" name="ESCAPE_CHARACTER" dataDxfId="142"/>
+    <tableColumn id="28" xr3:uid="{B74F90B2-DAF7-B94F-8284-1EEA400EF1FB}" name="DATE_FORMAT" dataDxfId="141"/>
+    <tableColumn id="35" xr3:uid="{03B4F8A1-AD12-8341-A343-173B2E180299}" name="DATETIME_FORMAT" dataDxfId="140"/>
+    <tableColumn id="36" xr3:uid="{DABEE994-4152-4DD6-ABEC-EB95AD8FE941}" name="FEED_RELEVANCE" dataDxfId="139"/>
+    <tableColumn id="38" xr3:uid="{78F40883-259F-1949-8F96-1FAFC8B1302C}" name="ENCRYPTED" dataDxfId="138"/>
+    <tableColumn id="26" xr3:uid="{420FC220-FD78-47EB-971E-A87F3D459433}" name="ESTIMATED_VOLUME_IN_GB" dataDxfId="137"/>
+    <tableColumn id="1" xr3:uid="{9F60E835-17EA-402E-BE58-F664166419BB}" name="PROMO" dataDxfId="136"/>
+    <tableColumn id="24" xr3:uid="{05342558-0B99-49EA-816A-D0DF857E4361}" name="PRICE" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1815171419" displayName="Table1815171419" ref="A1:Q475" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107">
-  <autoFilter ref="A1:Q475" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1815171419" displayName="Table1815171419" ref="A1:Q476" totalsRowShown="0" headerRowDxfId="134" dataDxfId="132" headerRowBorderDxfId="133">
+  <autoFilter ref="A1:Q476" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="FEED_TYPE" dataDxfId="105">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="FEED_TYPE" dataDxfId="131">
       <calculatedColumnFormula>INDEX('Feeds summary'!A:A,MATCH(Table1815171419[[#This Row],[SOURCE_FEED_NAME]],'Feeds summary'!C:C,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{41DC07BF-832B-40B5-9AAD-8FA634762071}" name="FEED_ID" dataDxfId="104">
+    <tableColumn id="17" xr3:uid="{41DC07BF-832B-40B5-9AAD-8FA634762071}" name="FEED_ID" dataDxfId="130">
       <calculatedColumnFormula>INDEX('Feeds summary'!B:B,MATCH(Table1815171419[[#This Row],[SOURCE_FEED_NAME]],'Feeds summary'!C:C,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0BC3BC73-81F8-4714-964B-619C28BA2848}" name="SOURCE_FEED_NAME" dataDxfId="103"/>
-    <tableColumn id="33" xr3:uid="{75AD7116-0B36-412B-BE85-C97786ACA0E2}" name="STAGE TABLE NAME" dataDxfId="102">
+    <tableColumn id="9" xr3:uid="{0BC3BC73-81F8-4714-964B-619C28BA2848}" name="SOURCE_FEED_NAME" dataDxfId="129"/>
+    <tableColumn id="33" xr3:uid="{75AD7116-0B36-412B-BE85-C97786ACA0E2}" name="STAGE TABLE NAME" dataDxfId="128">
       <calculatedColumnFormula>"T_"&amp;Table1815171419[[#This Row],[SOURCE_FEED_NAME]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{7623AE9D-5EB7-4872-8126-A2F7873CA41A}" name="SOURCE_COLUMN_NAME" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="TARGET_COLUMN_NAME" dataDxfId="100"/>
-    <tableColumn id="24" xr3:uid="{F94A8852-4A38-435F-B850-8066A4DD8972}" name="DESCRIPTION" dataDxfId="99"/>
-    <tableColumn id="25" xr3:uid="{D71B3972-6900-4FC1-81C6-43E59F45488E}" name="TARGET_COLUMN_DATA_TYPE" dataDxfId="98"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="COLUMN_ORDER" dataDxfId="97"/>
-    <tableColumn id="19" xr3:uid="{4FA1C0A8-DC6A-4E73-A175-F239B99012F5}" name="EXAMPLE_VALUES" dataDxfId="96"/>
-    <tableColumn id="35" xr3:uid="{001E2931-59BE-4BB8-BC09-BEF4D917CCB4}" name="NULLABLE" dataDxfId="95"/>
-    <tableColumn id="23" xr3:uid="{B4F894BC-7D13-48C9-AE4A-D8CB467601E7}" name="PRIMARY_KEY" dataDxfId="94"/>
-    <tableColumn id="36" xr3:uid="{764156E0-6BE1-4E6F-80F4-666197EE76E9}" name="INCREMENTALITY_KEY" dataDxfId="93"/>
-    <tableColumn id="22" xr3:uid="{B6F761AD-05E1-D843-9BFB-7D42140D4780}" name="FOREIGN_KEY_FEED_NAME" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{21D29095-5738-CB48-9CD1-74E3510BFA88}" name="FOREIGN_KEY_COLUMN_NAME" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{2E46A309-5087-4564-B0EA-E4CB0D4C0E27}" name="PRICE" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{E81906DE-E2D4-4B65-AA65-969F63F8E2D0}" name="PROMO" dataDxfId="89"/>
+    <tableColumn id="34" xr3:uid="{7623AE9D-5EB7-4872-8126-A2F7873CA41A}" name="SOURCE_COLUMN_NAME" dataDxfId="127"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="TARGET_COLUMN_NAME" dataDxfId="126"/>
+    <tableColumn id="24" xr3:uid="{F94A8852-4A38-435F-B850-8066A4DD8972}" name="DESCRIPTION" dataDxfId="125"/>
+    <tableColumn id="25" xr3:uid="{D71B3972-6900-4FC1-81C6-43E59F45488E}" name="TARGET_COLUMN_DATA_TYPE" dataDxfId="124"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="COLUMN_ORDER" dataDxfId="123"/>
+    <tableColumn id="19" xr3:uid="{4FA1C0A8-DC6A-4E73-A175-F239B99012F5}" name="EXAMPLE_VALUES" dataDxfId="122"/>
+    <tableColumn id="35" xr3:uid="{001E2931-59BE-4BB8-BC09-BEF4D917CCB4}" name="NULLABLE" dataDxfId="121"/>
+    <tableColumn id="23" xr3:uid="{B4F894BC-7D13-48C9-AE4A-D8CB467601E7}" name="PRIMARY_KEY" dataDxfId="120"/>
+    <tableColumn id="36" xr3:uid="{764156E0-6BE1-4E6F-80F4-666197EE76E9}" name="INCREMENTALITY_KEY" dataDxfId="119"/>
+    <tableColumn id="22" xr3:uid="{B6F761AD-05E1-D843-9BFB-7D42140D4780}" name="FOREIGN_KEY_FEED_NAME" dataDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{21D29095-5738-CB48-9CD1-74E3510BFA88}" name="FOREIGN_KEY_COLUMN_NAME" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{2E46A309-5087-4564-B0EA-E4CB0D4C0E27}" name="PRICE" dataDxfId="116"/>
+    <tableColumn id="5" xr3:uid="{E81906DE-E2D4-4B65-AA65-969F63F8E2D0}" name="PROMO" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{55F3FB13-315E-44A5-B01B-64EF8B13DC8A}" name="Table181517141978" displayName="Table181517141978" ref="A1:O475" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{55F3FB13-315E-44A5-B01B-64EF8B13DC8A}" name="Table181517141978" displayName="Table181517141978" ref="A1:O475" totalsRowShown="0" headerRowDxfId="114" dataDxfId="112" headerRowBorderDxfId="113">
   <autoFilter ref="A1:O475" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}">
     <filterColumn colId="0">
       <filters>
@@ -8565,30 +8595,30 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{730427C0-87C0-47B1-B30E-A52160573487}" name="Stage Table Name" dataDxfId="71"/>
-    <tableColumn id="33" xr3:uid="{3417A29B-6E81-446A-9183-85ECB22D2017}" name="PSA TABLE NAME" dataDxfId="70">
+    <tableColumn id="9" xr3:uid="{730427C0-87C0-47B1-B30E-A52160573487}" name="Stage Table Name" dataDxfId="111"/>
+    <tableColumn id="33" xr3:uid="{3417A29B-6E81-446A-9183-85ECB22D2017}" name="PSA TABLE NAME" dataDxfId="110">
       <calculatedColumnFormula>"T_"&amp;Table181517141978[[#This Row],[Stage Table Name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{0F436A2A-915A-4279-BD16-1C2E85B3B9F7}" name="SOURCE_COLUMN_NAME" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{FE8BA81A-BEF7-4D7A-8585-19BF308DD051}" name="TARGET_COLUMN_NAME" dataDxfId="68"/>
-    <tableColumn id="24" xr3:uid="{16D416D3-3D07-472C-9DF6-4B0C84E47BD6}" name="DESCRIPTION" dataDxfId="67"/>
-    <tableColumn id="25" xr3:uid="{3A05A57E-DB34-412F-90FD-0F95C0096970}" name="TARGET_COLUMN_DATA_TYPE" dataDxfId="66"/>
-    <tableColumn id="16" xr3:uid="{FB38957C-C746-40EC-AF52-9D8846C774C3}" name="COLUMN_ORDER" dataDxfId="65"/>
-    <tableColumn id="19" xr3:uid="{BD70F0B9-8A42-4E92-A625-7BAAD5398BC0}" name="EXAMPLE_VALUES" dataDxfId="64"/>
-    <tableColumn id="35" xr3:uid="{61F05D3D-94FD-46D6-B867-8374A41EDE01}" name="NULLABLE" dataDxfId="63"/>
-    <tableColumn id="23" xr3:uid="{5C4AE84A-E7BA-4DEA-8000-4A6CD0161600}" name="PRIMARY_KEY" dataDxfId="62"/>
-    <tableColumn id="36" xr3:uid="{6428F9A5-B92C-4823-99E5-2E19AA0F9A4C}" name="INCREMENTALITY_KEY" dataDxfId="61"/>
-    <tableColumn id="22" xr3:uid="{F68846EE-FCFF-4CAB-B02C-7A1F11097DB6}" name="FOREIGN_KEY_FEED_NAME" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{72BDE85A-0FA0-43E2-942D-1102046FDF9F}" name="FOREIGN_KEY_COLUMN_NAME" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{26043ECB-3050-43E4-9D1F-10DE36CD9CD2}" name="PRICE" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{D9480853-2A4A-42B8-8110-701438EA6CC0}" name="PROMO" dataDxfId="57"/>
+    <tableColumn id="34" xr3:uid="{0F436A2A-915A-4279-BD16-1C2E85B3B9F7}" name="SOURCE_COLUMN_NAME" dataDxfId="109"/>
+    <tableColumn id="6" xr3:uid="{FE8BA81A-BEF7-4D7A-8585-19BF308DD051}" name="TARGET_COLUMN_NAME" dataDxfId="108"/>
+    <tableColumn id="24" xr3:uid="{16D416D3-3D07-472C-9DF6-4B0C84E47BD6}" name="DESCRIPTION" dataDxfId="107"/>
+    <tableColumn id="25" xr3:uid="{3A05A57E-DB34-412F-90FD-0F95C0096970}" name="TARGET_COLUMN_DATA_TYPE" dataDxfId="106"/>
+    <tableColumn id="16" xr3:uid="{FB38957C-C746-40EC-AF52-9D8846C774C3}" name="COLUMN_ORDER" dataDxfId="105"/>
+    <tableColumn id="19" xr3:uid="{BD70F0B9-8A42-4E92-A625-7BAAD5398BC0}" name="EXAMPLE_VALUES" dataDxfId="104"/>
+    <tableColumn id="35" xr3:uid="{61F05D3D-94FD-46D6-B867-8374A41EDE01}" name="NULLABLE" dataDxfId="103"/>
+    <tableColumn id="23" xr3:uid="{5C4AE84A-E7BA-4DEA-8000-4A6CD0161600}" name="PRIMARY_KEY" dataDxfId="102"/>
+    <tableColumn id="36" xr3:uid="{6428F9A5-B92C-4823-99E5-2E19AA0F9A4C}" name="INCREMENTALITY_KEY" dataDxfId="101"/>
+    <tableColumn id="22" xr3:uid="{F68846EE-FCFF-4CAB-B02C-7A1F11097DB6}" name="FOREIGN_KEY_FEED_NAME" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{72BDE85A-0FA0-43E2-942D-1102046FDF9F}" name="FOREIGN_KEY_COLUMN_NAME" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{26043ECB-3050-43E4-9D1F-10DE36CD9CD2}" name="PRICE" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{D9480853-2A4A-42B8-8110-701438EA6CC0}" name="PROMO" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3A8FFC19-7406-4231-A665-178A26B52903}" name="Table18151714197" displayName="Table18151714197" ref="A1:O475" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3A8FFC19-7406-4231-A665-178A26B52903}" name="Table18151714197" displayName="Table18151714197" ref="A1:O475" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95">
   <autoFilter ref="A1:O475" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}">
     <filterColumn colId="0">
       <filters>
@@ -8597,48 +8627,48 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{1BD48EE7-BA46-4AC4-B75F-74AB0C5429BE}" name="PSA TABLE NAME" dataDxfId="39"/>
-    <tableColumn id="33" xr3:uid="{5E7D34C9-CD60-4F59-A3D1-4D5C3A03E3C4}" name="DWH TABLE NAME" dataDxfId="38">
+    <tableColumn id="9" xr3:uid="{1BD48EE7-BA46-4AC4-B75F-74AB0C5429BE}" name="PSA TABLE NAME" dataDxfId="93"/>
+    <tableColumn id="33" xr3:uid="{5E7D34C9-CD60-4F59-A3D1-4D5C3A03E3C4}" name="DWH TABLE NAME" dataDxfId="92">
       <calculatedColumnFormula>"T_"&amp;Table18151714197[[#This Row],[PSA TABLE NAME]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{A8A5C9E3-76C8-4B05-B2CB-24A9A23F0852}" name="SOURCE_COLUMN_NAME" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{FD4240FF-8C7B-4B4F-AD07-229E8A61367C}" name="TARGET_COLUMN_NAME" dataDxfId="36"/>
-    <tableColumn id="24" xr3:uid="{3BC8B01F-412A-44FE-9714-386082BE05C6}" name="DESCRIPTION" dataDxfId="35"/>
-    <tableColumn id="25" xr3:uid="{868C27B1-97E1-47BA-97DB-9D41E94C2FD7}" name="TARGET_COLUMN_DATA_TYPE" dataDxfId="34"/>
-    <tableColumn id="16" xr3:uid="{55EC57F6-0FCD-4E98-BCC3-8E4A5E5D6BFB}" name="COLUMN_ORDER" dataDxfId="33"/>
-    <tableColumn id="19" xr3:uid="{6554202A-70FC-4671-B25F-1AF4BB9058FB}" name="EXAMPLE_VALUES" dataDxfId="32"/>
-    <tableColumn id="35" xr3:uid="{6877C0D5-D695-44FB-8FE2-69CA94A92102}" name="NULLABLE" dataDxfId="31"/>
-    <tableColumn id="23" xr3:uid="{3B348965-C262-4FD6-A9C3-C7107D616DA0}" name="PRIMARY_KEY" dataDxfId="30"/>
-    <tableColumn id="36" xr3:uid="{110B2688-29DD-4DF1-99E5-1F06703E57E7}" name="INCREMENTALITY_KEY" dataDxfId="29"/>
-    <tableColumn id="22" xr3:uid="{E293CBD8-F543-444C-A582-01D9771A3141}" name="FOREIGN_KEY_FEED_NAME" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{089276C7-CB7C-49F1-BBA9-CA5B03261AD3}" name="FOREIGN_KEY_COLUMN_NAME" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{5BD51AD1-AE3A-478E-BC43-0AA73CBA8085}" name="PRICE" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{0A246595-B61E-4CFC-B88E-EF60C7073DA9}" name="PROMO" dataDxfId="25"/>
+    <tableColumn id="34" xr3:uid="{A8A5C9E3-76C8-4B05-B2CB-24A9A23F0852}" name="SOURCE_COLUMN_NAME" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{FD4240FF-8C7B-4B4F-AD07-229E8A61367C}" name="TARGET_COLUMN_NAME" dataDxfId="90"/>
+    <tableColumn id="24" xr3:uid="{3BC8B01F-412A-44FE-9714-386082BE05C6}" name="DESCRIPTION" dataDxfId="89"/>
+    <tableColumn id="25" xr3:uid="{868C27B1-97E1-47BA-97DB-9D41E94C2FD7}" name="TARGET_COLUMN_DATA_TYPE" dataDxfId="88"/>
+    <tableColumn id="16" xr3:uid="{55EC57F6-0FCD-4E98-BCC3-8E4A5E5D6BFB}" name="COLUMN_ORDER" dataDxfId="87"/>
+    <tableColumn id="19" xr3:uid="{6554202A-70FC-4671-B25F-1AF4BB9058FB}" name="EXAMPLE_VALUES" dataDxfId="86"/>
+    <tableColumn id="35" xr3:uid="{6877C0D5-D695-44FB-8FE2-69CA94A92102}" name="NULLABLE" dataDxfId="85"/>
+    <tableColumn id="23" xr3:uid="{3B348965-C262-4FD6-A9C3-C7107D616DA0}" name="PRIMARY_KEY" dataDxfId="84"/>
+    <tableColumn id="36" xr3:uid="{110B2688-29DD-4DF1-99E5-1F06703E57E7}" name="INCREMENTALITY_KEY" dataDxfId="83"/>
+    <tableColumn id="22" xr3:uid="{E293CBD8-F543-444C-A582-01D9771A3141}" name="FOREIGN_KEY_FEED_NAME" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{089276C7-CB7C-49F1-BBA9-CA5B03261AD3}" name="FOREIGN_KEY_COLUMN_NAME" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{5BD51AD1-AE3A-478E-BC43-0AA73CBA8085}" name="PRICE" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{0A246595-B61E-4CFC-B88E-EF60C7073DA9}" name="PROMO" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A6D9F89-9D54-1D4A-9F32-C3C93801C085}" name="Table3" displayName="Table3" ref="B4:E44" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A6D9F89-9D54-1D4A-9F32-C3C93801C085}" name="Table3" displayName="Table3" ref="B4:E44" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17CD7601-6A6D-F145-A5E5-237E8B7BB97F}" name="Name" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{11AE440F-8CE1-BF49-A1F9-092CD206D2C2}" name="Definition" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{FC983F67-8CB0-0349-81CC-3C1C66452F6C}" name="Example" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{6EA95545-E727-EF48-AB0B-7442BF3CD9C7}" name="Allowed values" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{17CD7601-6A6D-F145-A5E5-237E8B7BB97F}" name="Name" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{11AE440F-8CE1-BF49-A1F9-092CD206D2C2}" name="Definition" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{FC983F67-8CB0-0349-81CC-3C1C66452F6C}" name="Example" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{6EA95545-E727-EF48-AB0B-7442BF3CD9C7}" name="Allowed values" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{98AC3462-778B-F745-ADED-AF22C75B8DFC}" name="Table4" displayName="Table4" ref="B49:E79" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{98AC3462-778B-F745-ADED-AF22C75B8DFC}" name="Table4" displayName="Table4" ref="B49:E79" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
   <autoFilter ref="B49:E79" xr:uid="{600A5B1E-0906-2540-8E97-7DA996358180}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F6F6C760-C09C-0646-83E7-264FB6DB7ABF}" name="Column name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{621888D6-A254-D545-94FC-17949618B0CC}" name="Description" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{589ED7DF-0048-614D-80FD-BD60A1373142}" name="Example" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{01250796-9AAB-C74B-8E90-B4AA23ACC1B9}" name="Allowed values" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{F6F6C760-C09C-0646-83E7-264FB6DB7ABF}" name="Column name" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{621888D6-A254-D545-94FC-17949618B0CC}" name="Description" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{589ED7DF-0048-614D-80FD-BD60A1373142}" name="Example" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{01250796-9AAB-C74B-8E90-B4AA23ACC1B9}" name="Allowed values" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8666,14 +8696,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D19797B0-3294-44B6-887D-C5F365DCEC43}" name="Table181517141915" displayName="Table181517141915" ref="A1:F155" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D19797B0-3294-44B6-887D-C5F365DCEC43}" name="Table181517141915" displayName="Table181517141915" ref="A1:F155" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C78013F0-A13F-420F-9C79-1B6893851CA0}" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{3A7A7FD0-6B61-46B7-80A1-5F2C1CBA3099}" name="Version #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{AD04A614-70E9-4812-9737-CCDC3C15895E}" name="Who" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A19639C0-8220-4824-921A-0302CC80D172}" name="What" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{04A4C0A2-6F6A-4461-9143-3CB1ACDF2E38}" name="Questions/Assumptions/Actions" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F78D122C-0DC4-4AFA-866A-F2E70B1A55F4}" name="Approved" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C78013F0-A13F-420F-9C79-1B6893851CA0}" name="Date" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{3A7A7FD0-6B61-46B7-80A1-5F2C1CBA3099}" name="Version #" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{AD04A614-70E9-4812-9737-CCDC3C15895E}" name="Who" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{A19639C0-8220-4824-921A-0302CC80D172}" name="What" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{04A4C0A2-6F6A-4461-9143-3CB1ACDF2E38}" name="Questions/Assumptions/Actions" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{F78D122C-0DC4-4AFA-866A-F2E70B1A55F4}" name="Approved" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10118,7 +10148,7 @@
       </c>
       <c r="F62" s="10"/>
     </row>
-    <row r="63" spans="1:6" ht="325.5">
+    <row r="63" spans="1:6" ht="341">
       <c r="A63" s="56">
         <v>43228</v>
       </c>
@@ -11752,7 +11782,7 @@
   <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="92" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
@@ -12316,7 +12346,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" ht="31">
       <c r="A7" s="8" t="s">
         <v>118</v>
       </c>
@@ -13125,50 +13155,50 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="AG1 AG2:AH3 AG4 AI4:AM8 AG5:AH6">
-    <cfRule type="cellIs" dxfId="173" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="109" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="110" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG7:AG8">
-    <cfRule type="cellIs" dxfId="171" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="8" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG9:AM1048576">
-    <cfRule type="cellIs" dxfId="169" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH1">
-    <cfRule type="cellIs" dxfId="167" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="45" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="46" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4">
-    <cfRule type="cellIs" dxfId="165" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH7:AH8">
-    <cfRule type="cellIs" dxfId="163" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="9" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13222,8 +13252,8 @@
   </sheetPr>
   <dimension ref="A1:Q569"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F384" sqref="F384"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A462" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D476" sqref="D476"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.83203125" defaultRowHeight="15.5"/>
@@ -32686,6 +32716,48 @@
       <c r="P475" s="10"/>
       <c r="Q475" s="10"/>
     </row>
+    <row r="476" spans="1:17">
+      <c r="A476" s="118" t="str">
+        <f>INDEX('Feeds summary'!A:A,MATCH(Table1815171419[[#This Row],[SOURCE_FEED_NAME]],'Feeds summary'!C:C,0))</f>
+        <v>CURRENCY</v>
+      </c>
+      <c r="B476" s="118">
+        <f>INDEX('Feeds summary'!B:B,MATCH(Table1815171419[[#This Row],[SOURCE_FEED_NAME]],'Feeds summary'!C:C,0))</f>
+        <v>6</v>
+      </c>
+      <c r="C476" s="119" t="s">
+        <v>118</v>
+      </c>
+      <c r="D476" s="118" t="str">
+        <f>"T_"&amp;Table1815171419[[#This Row],[SOURCE_FEED_NAME]]</f>
+        <v>T_CURRENCY</v>
+      </c>
+      <c r="E476" s="120"/>
+      <c r="F476" s="121" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G476" s="122" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H476" s="122" t="s">
+        <v>152</v>
+      </c>
+      <c r="I476" s="122">
+        <v>100</v>
+      </c>
+      <c r="J476" s="123"/>
+      <c r="K476" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="L476" s="122" t="s">
+        <v>35</v>
+      </c>
+      <c r="M476" s="122"/>
+      <c r="N476" s="122"/>
+      <c r="O476" s="122"/>
+      <c r="P476" s="118"/>
+      <c r="Q476" s="118"/>
+    </row>
     <row r="569" spans="1:17" s="7" customFormat="1">
       <c r="A569" s="1"/>
       <c r="B569" s="1"/>
@@ -32708,73 +32780,73 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="K322:K381">
-    <cfRule type="cellIs" dxfId="122" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="33" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:L243">
-    <cfRule type="cellIs" dxfId="121" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K382:L386">
-    <cfRule type="cellIs" dxfId="120" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="30" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:O1 K387:K388 O387:O1048576 K389:M394 M395:M396 K395:K397 K397:M411 M412:M1048576">
-    <cfRule type="cellIs" dxfId="119" priority="836" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="836" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244:O321">
-    <cfRule type="cellIs" dxfId="118" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L322:L381">
-    <cfRule type="cellIs" dxfId="117" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="31" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L387:L388">
-    <cfRule type="cellIs" dxfId="116" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L395:L396">
-    <cfRule type="cellIs" dxfId="115" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O243">
-    <cfRule type="cellIs" dxfId="114" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="18" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O322:O386 M322:M388">
-    <cfRule type="cellIs" dxfId="113" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:Q321">
-    <cfRule type="cellIs" dxfId="112" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R736:T1048576">
-    <cfRule type="cellIs" dxfId="110" priority="841" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="841" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="842" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="842" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O257:O1048576 M2:M475 K2:L411" xr:uid="{8B4E4464-E3EF-0144-8EC7-6CDCE807347D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O257:O1048576 M2:M476 K2:L411" xr:uid="{8B4E4464-E3EF-0144-8EC7-6CDCE807347D}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -48512,68 +48584,68 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I322:I381">
-    <cfRule type="cellIs" dxfId="88" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J243">
-    <cfRule type="cellIs" dxfId="87" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I382:J386">
-    <cfRule type="cellIs" dxfId="86" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:M1 I387:I388 M387:M1048576 I389:K394 K395:K396 I395:I411 J397:K411 K412:K1048576">
-    <cfRule type="cellIs" dxfId="85" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I244:M321">
-    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J322:J381">
-    <cfRule type="cellIs" dxfId="83" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J387:J388">
-    <cfRule type="cellIs" dxfId="82" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J395:J396">
-    <cfRule type="cellIs" dxfId="81" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:M243">
-    <cfRule type="cellIs" dxfId="80" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M322:M386 K322:K388">
-    <cfRule type="cellIs" dxfId="79" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O321">
-    <cfRule type="cellIs" dxfId="78" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P736:R1048576">
-    <cfRule type="cellIs" dxfId="76" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="38" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="39" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -64316,68 +64388,68 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I322:I381">
-    <cfRule type="cellIs" dxfId="56" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J243">
-    <cfRule type="cellIs" dxfId="55" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I382:J386">
-    <cfRule type="cellIs" dxfId="54" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:M1 I387:I388 M387:M1048576 I389:K394 K395:K396 I395:I411 J397:K411 K412:K1048576">
-    <cfRule type="cellIs" dxfId="53" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="37" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I244:M321">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J322:J381">
-    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J387:J388">
-    <cfRule type="cellIs" dxfId="50" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="23" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J395:J396">
-    <cfRule type="cellIs" dxfId="49" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:M243">
-    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M322:M386 K322:K388">
-    <cfRule type="cellIs" dxfId="47" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="33" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O321">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P736:R1048576">
-    <cfRule type="cellIs" dxfId="44" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="38" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="39" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -65438,7 +65510,7 @@
       </c>
       <c r="E66" s="54"/>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:5" ht="31">
       <c r="B67" s="70" t="s">
         <v>862</v>
       </c>
@@ -65616,18 +65688,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B35:B44">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70:B79">
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -65647,7 +65719,7 @@
   </sheetPr>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -65871,18 +65943,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66050,6 +66122,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40AFD744-41D8-41A8-815D-4FF1B99CB720}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F3AABC3-1842-460E-8E77-73AEFCFAE11E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -66061,14 +66141,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="ba1ea0db-fff4-400c-aea0-490a43c36365"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40AFD744-41D8-41A8-815D-4FF1B99CB720}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>